<commit_message>
LoadOfDisciplines. Save to online.edu
</commit_message>
<xml_diff>
--- a/Шаблон дисциплины.xlsx
+++ b/Шаблон дисциплины.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1\online.edu.loader\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D49DC8C-62DE-4374-A96F-407D38DCA5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,16 +40,40 @@
     <x:t>Название дисциплины</x:t>
   </x:si>
   <x:si>
-    <x:t>6a95941c-7b52-4e83-99bb-b7a4e884efc7</x:t>
+    <x:t>26cf7f91-ae41-424a-829d-2d7fdc8b2e25</x:t>
   </x:si>
   <x:si>
     <x:t>Основы электротехники</x:t>
   </x:si>
   <x:si>
-    <x:t>af06ef21-3cfe-4e42-bd8f-089210927fcb</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Заполняется программой</x:t>
+    <x:t>7d730da6-7397-404c-8c97-958a044ecac6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>a1cc46ec-1f3c-4869-aa53-8f5457a548e0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Тестова дисцеплина 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>b3d81cf2-3d21-48f3-8e75-9cb6d19ae8d2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>e6d8315c-1d9f-4acb-a7e3-cae1e46e3ce6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Тестова дисцеплина 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>90fd1985-565f-4438-9e01-c8762406d4e4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c02b9f8c-fe52-46dc-8a03-38a13596b438</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Тестова дисцеплина 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ce1475bc-076a-46b8-950a-cfb8f79e598b</x:t>
   </x:si>
   <x:si>
     <x:t>Возвращается программой</x:t>
@@ -52,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
@@ -195,21 +225,24 @@
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
-    <x:cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
   </x:extLst>
 </x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,9 +280,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,9 +315,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,9 +367,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -492,24 +559,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:C36"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <x:selection activeCell="E9" sqref="E9"/>
+      <x:selection activeCell="B14" sqref="B14"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="76.710938" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="30.285156" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="33.140625" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="30.425781" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="47.140625" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -520,7 +587,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A2" s="4" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -531,7 +598,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A3" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -542,301 +609,247 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A4" s="6" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B4" s="1"/>
+      <x:c r="B4" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
       <x:c r="C4" s="6" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A5" s="6" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B5" s="1"/>
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
       <x:c r="C5" s="6" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A6" s="6" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B6" s="1"/>
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B6" s="1" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="C6" s="6" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="1"/>
       <x:c r="B7" s="1"/>
       <x:c r="C7" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="1"/>
       <x:c r="B8" s="1"/>
       <x:c r="C8" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="1"/>
       <x:c r="B9" s="1"/>
       <x:c r="C9" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="1"/>
       <x:c r="B10" s="1"/>
       <x:c r="C10" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="1"/>
       <x:c r="B11" s="1"/>
       <x:c r="C11" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="1"/>
       <x:c r="B12" s="1"/>
       <x:c r="C12" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="1"/>
       <x:c r="B13" s="1"/>
       <x:c r="C13" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="1"/>
       <x:c r="B14" s="1"/>
       <x:c r="C14" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A15" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="1"/>
       <x:c r="B15" s="1"/>
       <x:c r="C15" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A16" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="1"/>
       <x:c r="B16" s="1"/>
       <x:c r="C16" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A17" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="1"/>
       <x:c r="B17" s="1"/>
       <x:c r="C17" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A18" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="1"/>
       <x:c r="B18" s="1"/>
       <x:c r="C18" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A19" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A19" s="1"/>
       <x:c r="B19" s="1"/>
       <x:c r="C19" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A20" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A20" s="1"/>
       <x:c r="B20" s="1"/>
       <x:c r="C20" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A21" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A21" s="1"/>
       <x:c r="B21" s="1"/>
       <x:c r="C21" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A22" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A22" s="1"/>
       <x:c r="B22" s="1"/>
       <x:c r="C22" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A23" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A23" s="1"/>
       <x:c r="B23" s="1"/>
       <x:c r="C23" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A24" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A24" s="1"/>
       <x:c r="B24" s="1"/>
       <x:c r="C24" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A25" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A25" s="1"/>
       <x:c r="B25" s="1"/>
       <x:c r="C25" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A26" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A26" s="1"/>
       <x:c r="B26" s="1"/>
       <x:c r="C26" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A27" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A27" s="1"/>
       <x:c r="B27" s="1"/>
       <x:c r="C27" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A28" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A28" s="1"/>
       <x:c r="B28" s="1"/>
       <x:c r="C28" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A29" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A29" s="1"/>
       <x:c r="B29" s="1"/>
       <x:c r="C29" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A30" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A30" s="1"/>
       <x:c r="B30" s="1"/>
       <x:c r="C30" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A31" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A31" s="1"/>
       <x:c r="B31" s="1"/>
       <x:c r="C31" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A32" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A32" s="1"/>
       <x:c r="B32" s="1"/>
       <x:c r="C32" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A33" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A33" s="1"/>
       <x:c r="B33" s="1"/>
       <x:c r="C33" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A34" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A34" s="1"/>
       <x:c r="B34" s="1"/>
       <x:c r="C34" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A35" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A35" s="1"/>
       <x:c r="B35" s="1"/>
       <x:c r="C35" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A36" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A36" s="1"/>
       <x:c r="B36" s="1"/>
       <x:c r="C36" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -849,7 +862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -868,7 +881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>

</xml_diff>